<commit_message>
Update: Input as byte array and change response form LLM
</commit_message>
<xml_diff>
--- a/output/Trade_Confirmation_extracted.xlsx
+++ b/output/Trade_Confirmation_extracted.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Extracted Fields" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Field Metadata" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +18,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +38,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +46,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -511,11 +524,7 @@
           <t>Currency</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Company Name or Bank Name</t>
-        </is>
-      </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -564,6 +573,457 @@
           <t>XYZ</t>
         </is>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Field</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>RowIndex</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>start_index_nbr</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>end_index_nbr</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>row_adder_cnt</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>col_adder_cnt</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>param_ref_delim_txt</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>param_value_pos_cd</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>unit_price_pct_ind</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>param_nm_occur_ind</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>date_format_cd</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>decimal_separator_cd</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>param_def_value_txt</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>derivation_col</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>operations_seq</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Trade Date</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>295</v>
+      </c>
+      <c r="D2" t="n">
+        <v>311</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Month DD, YYYY</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Settlement Date</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>322</v>
+      </c>
+      <c r="D3" t="n">
+        <v>342</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Month DD, YYYY</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Transaction Type</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Buyer and Seller</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>inferred from roles</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Net Amount or Consideration Amount or Nominal Amount</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>494</v>
+      </c>
+      <c r="D5" t="n">
+        <v>512</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Unit Price or Price</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>523</v>
+      </c>
+      <c r="D6" t="n">
+        <v>529</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Units or Shares</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ISIN or RIC</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>473</v>
+      </c>
+      <c r="D8" t="n">
+        <v>483</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>453</v>
+      </c>
+      <c r="D9" t="n">
+        <v>462</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Company Name or Bank Name</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Buyer</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>